<commit_message>
finished experimentation again and results
</commit_message>
<xml_diff>
--- a/reports/manual_tables_and_charts.xlsx
+++ b/reports/manual_tables_and_charts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicole.r.frank/Projects/credit-decisioning/reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE7E63E1-E4B5-F44B-B0BC-DB8D750BE7C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B974B4-6221-7E41-80FB-C4E5857F4E8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="900" windowWidth="28040" windowHeight="17180" xr2:uid="{C45BFEA9-A238-3B48-B16D-41F98FACE761}"/>
+    <workbookView xWindow="31080" yWindow="3840" windowWidth="25760" windowHeight="14960" xr2:uid="{C45BFEA9-A238-3B48-B16D-41F98FACE761}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="3" r:id="rId1"/>
@@ -285,10 +285,10 @@
     <t>Loan_status Distribution Combined</t>
   </si>
   <si>
-    <t>Good CD</t>
-  </si>
-  <si>
-    <t>Bad CD</t>
+    <t>Good Credit Decision</t>
+  </si>
+  <si>
+    <t>Bad Credit Decision</t>
   </si>
 </sst>
 </file>
@@ -1038,10 +1038,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>Good CD</c:v>
+                  <c:v>Good Credit Decision</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Bad CD</c:v>
+                  <c:v>Bad Credit Decision</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2723,7 +2723,7 @@
   <dimension ref="B3:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>